<commit_message>
added intermediate pickles and updated scope3 xlsx file
</commit_message>
<xml_diff>
--- a/import_data/Scope 3 Emissions Factors.xlsx
+++ b/import_data/Scope 3 Emissions Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{8F4AF713-8A4C-4592-B1D8-6EA6215F16D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82B5F934-331B-47BE-B418-5681A79DE411}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{8F4AF713-8A4C-4592-B1D8-6EA6215F16D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AD5955E-43DB-457F-8B85-E80D1C66923C}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" xr2:uid="{20B9AD7C-31DE-49D1-ABBE-CD36CEC5113E}"/>
+    <workbookView xWindow="4510" yWindow="-16110" windowWidth="25820" windowHeight="15620" xr2:uid="{20B9AD7C-31DE-49D1-ABBE-CD36CEC5113E}"/>
   </bookViews>
   <sheets>
     <sheet name="Scope 3 EF" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>Met coal</t>
   </si>
   <si>
-    <t>Therm coal</t>
-  </si>
-  <si>
     <t>Slag</t>
   </si>
   <si>
@@ -84,12 +81,15 @@
   <si>
     <t>Slag [ton CO2eq/ton Slag]</t>
   </si>
+  <si>
+    <t>Thermal coal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,18 +513,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246167E3-ABFA-4DF2-BDC9-BE8A0DFB3E24}">
   <dimension ref="A1:AH6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:AH4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.9375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="1" customFormat="1">
+    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,7 +628,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -732,7 +732,7 @@
         <v>2.9723991507430998E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -836,7 +836,7 @@
         <v>1.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -971,12 +971,12 @@
         <v>1.277584E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1075,15 +1075,15 @@
         <v>1.277584E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
       </c>
       <c r="D6">
         <f>Assumptions!$B$6*Assumptions!C3</f>
@@ -1224,15 +1224,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" s="1" customFormat="1">
+    <row r="2" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -1329,9 +1329,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.5">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6">
@@ -1428,17 +1428,17 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>0.55000000000000004</v>
@@ -1450,12 +1450,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="f6f44a7d-d6f5-4042-8792-19cb5f90fb06">
+      <UserInfo>
+        <DisplayName>Andrew Isabirye</DisplayName>
+        <AccountId>30706</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1624,27 +1629,47 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="f6f44a7d-d6f5-4042-8792-19cb5f90fb06">
-      <UserInfo>
-        <DisplayName>Andrew Isabirye</DisplayName>
-        <AccountId>30706</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9009A692-B4CA-498A-A10B-38BC29B1B69F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1DA6178-4AFE-4392-812F-6E8389CD2EED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8E4E13-DB0E-424C-86A0-0473D26620F3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8E4E13-DB0E-424C-86A0-0473D26620F3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b44fa922-a688-4301-8945-67f7597c9c55"/>
+    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1DA6178-4AFE-4392-812F-6E8389CD2EED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9009A692-B4CA-498A-A10B-38BC29B1B69F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>